<commit_message>
Update based on change in analysis plan
</commit_message>
<xml_diff>
--- a/REACH_CAR_MSNA_DataAnalysisPlan_Indicators_July2019_HH_KI_FINAL_em.XLSX
+++ b/REACH_CAR_MSNA_DataAnalysisPlan_Indicators_July2019_HH_KI_FINAL_em.XLSX
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elliott Messeiller\Documents\SpiderOak Hive\IMPACT\26_CAR\MSNA_KIIsAgregation\CAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elliott Messeiller\Documents\SpiderOak Hive\IMPACT\26_CAR\MSNA_KIIsAgregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4654,9 +4654,6 @@
     <t>Choix multiple: Toutes les réponses sont égales (pondération modale)</t>
   </si>
   <si>
-    <t>Sélectionner la réponse la plus récente</t>
-  </si>
-  <si>
     <t>Toutes les réponses sont égales (pondération modale)</t>
   </si>
   <si>
@@ -4667,6 +4664,9 @@
   </si>
   <si>
     <t>Oui &gt; toutes les autres réponses</t>
+  </si>
+  <si>
+    <t>Pas suffisant du tout &gt; Insuffisant &gt; toute autre réponse</t>
   </si>
 </sst>
 </file>
@@ -5553,7 +5553,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -5878,349 +5878,352 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6608,13 +6611,13 @@
       <c r="K1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="L1" s="193" t="s">
+      <c r="L1" s="151" t="s">
         <v>185</v>
       </c>
-      <c r="M1" s="193"/>
-      <c r="N1" s="193"/>
-      <c r="O1" s="193"/>
-      <c r="P1" s="193"/>
+      <c r="M1" s="151"/>
+      <c r="N1" s="151"/>
+      <c r="O1" s="151"/>
+      <c r="P1" s="151"/>
     </row>
     <row r="2" spans="1:16" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6946,11 +6949,11 @@
       <c r="K13" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="L13" s="132"/>
-      <c r="M13" s="133"/>
-      <c r="N13" s="133"/>
-      <c r="O13" s="134"/>
-      <c r="P13" s="138" t="s">
+      <c r="L13" s="207"/>
+      <c r="M13" s="208"/>
+      <c r="N13" s="208"/>
+      <c r="O13" s="209"/>
+      <c r="P13" s="213" t="s">
         <v>528</v>
       </c>
     </row>
@@ -6988,11 +6991,11 @@
       <c r="K14" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="L14" s="135"/>
-      <c r="M14" s="136"/>
-      <c r="N14" s="136"/>
-      <c r="O14" s="137"/>
-      <c r="P14" s="139"/>
+      <c r="L14" s="210"/>
+      <c r="M14" s="211"/>
+      <c r="N14" s="211"/>
+      <c r="O14" s="212"/>
+      <c r="P14" s="214"/>
     </row>
     <row r="15" spans="1:16" ht="115.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -7617,10 +7620,10 @@
       <c r="N29" s="36" t="s">
         <v>204</v>
       </c>
-      <c r="O29" s="140" t="s">
+      <c r="O29" s="143" t="s">
         <v>516</v>
       </c>
-      <c r="P29" s="141"/>
+      <c r="P29" s="145"/>
     </row>
     <row r="30" spans="1:16" ht="77.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
@@ -7658,13 +7661,13 @@
       <c r="K30" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="L30" s="171" t="s">
+      <c r="L30" s="140" t="s">
         <v>201</v>
       </c>
-      <c r="M30" s="172"/>
-      <c r="N30" s="172"/>
-      <c r="O30" s="172"/>
-      <c r="P30" s="173"/>
+      <c r="M30" s="141"/>
+      <c r="N30" s="141"/>
+      <c r="O30" s="141"/>
+      <c r="P30" s="142"/>
     </row>
     <row r="31" spans="1:16" ht="131.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
@@ -7702,11 +7705,11 @@
       <c r="K31" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="L31" s="174"/>
-      <c r="M31" s="175"/>
-      <c r="N31" s="175"/>
-      <c r="O31" s="175"/>
-      <c r="P31" s="176"/>
+      <c r="L31" s="170"/>
+      <c r="M31" s="171"/>
+      <c r="N31" s="171"/>
+      <c r="O31" s="171"/>
+      <c r="P31" s="172"/>
     </row>
     <row r="32" spans="1:16" ht="156" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
@@ -7744,19 +7747,19 @@
       <c r="K32" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="L32" s="154" t="s">
+      <c r="L32" s="129" t="s">
         <v>463</v>
       </c>
-      <c r="M32" s="152" t="s">
+      <c r="M32" s="127" t="s">
         <v>466</v>
       </c>
-      <c r="N32" s="150" t="s">
+      <c r="N32" s="137" t="s">
         <v>467</v>
       </c>
-      <c r="O32" s="142" t="s">
+      <c r="O32" s="135" t="s">
         <v>464</v>
       </c>
-      <c r="P32" s="125" t="s">
+      <c r="P32" s="149" t="s">
         <v>465</v>
       </c>
     </row>
@@ -7796,11 +7799,11 @@
       <c r="K33" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="L33" s="155"/>
-      <c r="M33" s="153"/>
-      <c r="N33" s="151"/>
-      <c r="O33" s="144"/>
-      <c r="P33" s="127"/>
+      <c r="L33" s="219"/>
+      <c r="M33" s="218"/>
+      <c r="N33" s="139"/>
+      <c r="O33" s="199"/>
+      <c r="P33" s="200"/>
     </row>
     <row r="34" spans="1:16" ht="67.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
@@ -7838,12 +7841,12 @@
       <c r="K34" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="L34" s="147" t="s">
+      <c r="L34" s="133" t="s">
         <v>218</v>
       </c>
-      <c r="M34" s="148"/>
-      <c r="N34" s="148"/>
-      <c r="O34" s="149"/>
+      <c r="M34" s="205"/>
+      <c r="N34" s="205"/>
+      <c r="O34" s="134"/>
       <c r="P34" s="38" t="s">
         <v>217</v>
       </c>
@@ -7884,14 +7887,14 @@
       <c r="K35" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="L35" s="147" t="s">
+      <c r="L35" s="133" t="s">
         <v>219</v>
       </c>
-      <c r="M35" s="148"/>
-      <c r="N35" s="148" t="s">
+      <c r="M35" s="205"/>
+      <c r="N35" s="205" t="s">
         <v>206</v>
       </c>
-      <c r="O35" s="149" t="s">
+      <c r="O35" s="134" t="s">
         <v>207</v>
       </c>
       <c r="P35" s="38" t="s">
@@ -8038,13 +8041,13 @@
       <c r="K38" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="L38" s="156" t="s">
+      <c r="L38" s="220" t="s">
         <v>201</v>
       </c>
-      <c r="M38" s="157"/>
-      <c r="N38" s="157"/>
-      <c r="O38" s="157"/>
-      <c r="P38" s="158"/>
+      <c r="M38" s="221"/>
+      <c r="N38" s="221"/>
+      <c r="O38" s="221"/>
+      <c r="P38" s="222"/>
     </row>
     <row r="39" spans="1:16" ht="156.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
@@ -8082,17 +8085,17 @@
       <c r="K39" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="L39" s="116" t="s">
+      <c r="L39" s="178" t="s">
         <v>229</v>
       </c>
-      <c r="M39" s="118"/>
-      <c r="N39" s="150" t="s">
+      <c r="M39" s="179"/>
+      <c r="N39" s="137" t="s">
         <v>478</v>
       </c>
-      <c r="O39" s="185" t="s">
+      <c r="O39" s="125" t="s">
         <v>479</v>
       </c>
-      <c r="P39" s="186"/>
+      <c r="P39" s="126"/>
     </row>
     <row r="40" spans="1:16" ht="192" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
@@ -8130,9 +8133,9 @@
       <c r="K40" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="L40" s="122"/>
-      <c r="M40" s="124"/>
-      <c r="N40" s="151"/>
+      <c r="L40" s="185"/>
+      <c r="M40" s="186"/>
+      <c r="N40" s="139"/>
       <c r="O40" s="187"/>
       <c r="P40" s="188"/>
     </row>
@@ -8318,19 +8321,19 @@
       <c r="K44" s="79" t="s">
         <v>173</v>
       </c>
-      <c r="L44" s="207" t="s">
+      <c r="L44" s="180" t="s">
         <v>369</v>
       </c>
-      <c r="M44" s="159" t="s">
+      <c r="M44" s="166" t="s">
         <v>370</v>
       </c>
-      <c r="N44" s="161" t="s">
+      <c r="N44" s="164" t="s">
         <v>371</v>
       </c>
-      <c r="O44" s="128" t="s">
+      <c r="O44" s="162" t="s">
         <v>373</v>
       </c>
-      <c r="P44" s="130" t="s">
+      <c r="P44" s="160" t="s">
         <v>372</v>
       </c>
     </row>
@@ -8370,7 +8373,7 @@
       <c r="K45" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="L45" s="208"/>
+      <c r="L45" s="181"/>
       <c r="M45" s="192"/>
       <c r="N45" s="191"/>
       <c r="O45" s="190"/>
@@ -8410,19 +8413,19 @@
       <c r="K46" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="L46" s="117" t="s">
+      <c r="L46" s="168" t="s">
         <v>200</v>
       </c>
-      <c r="M46" s="159" t="s">
+      <c r="M46" s="166" t="s">
         <v>199</v>
       </c>
-      <c r="N46" s="161" t="s">
+      <c r="N46" s="164" t="s">
         <v>198</v>
       </c>
-      <c r="O46" s="128" t="s">
+      <c r="O46" s="162" t="s">
         <v>197</v>
       </c>
-      <c r="P46" s="130" t="s">
+      <c r="P46" s="160" t="s">
         <v>196</v>
       </c>
     </row>
@@ -8460,11 +8463,11 @@
       <c r="K47" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="L47" s="120"/>
-      <c r="M47" s="160"/>
-      <c r="N47" s="162"/>
-      <c r="O47" s="129"/>
-      <c r="P47" s="131"/>
+      <c r="L47" s="169"/>
+      <c r="M47" s="167"/>
+      <c r="N47" s="165"/>
+      <c r="O47" s="163"/>
+      <c r="P47" s="161"/>
     </row>
     <row r="48" spans="1:16" ht="115.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
@@ -8502,19 +8505,19 @@
       <c r="K48" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="L48" s="117" t="s">
+      <c r="L48" s="168" t="s">
         <v>485</v>
       </c>
-      <c r="M48" s="159" t="s">
+      <c r="M48" s="166" t="s">
         <v>486</v>
       </c>
-      <c r="N48" s="161" t="s">
+      <c r="N48" s="164" t="s">
         <v>486</v>
       </c>
-      <c r="O48" s="128" t="s">
+      <c r="O48" s="162" t="s">
         <v>487</v>
       </c>
-      <c r="P48" s="130" t="s">
+      <c r="P48" s="160" t="s">
         <v>488</v>
       </c>
     </row>
@@ -8554,11 +8557,11 @@
       <c r="K49" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="L49" s="120"/>
-      <c r="M49" s="160"/>
-      <c r="N49" s="162"/>
-      <c r="O49" s="129"/>
-      <c r="P49" s="131"/>
+      <c r="L49" s="169"/>
+      <c r="M49" s="167"/>
+      <c r="N49" s="165"/>
+      <c r="O49" s="163"/>
+      <c r="P49" s="161"/>
     </row>
     <row r="50" spans="1:16" ht="115.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
@@ -8691,12 +8694,12 @@
       <c r="L52" s="87" t="s">
         <v>381</v>
       </c>
-      <c r="M52" s="145" t="s">
+      <c r="M52" s="216" t="s">
         <v>382</v>
       </c>
-      <c r="N52" s="145"/>
-      <c r="O52" s="145"/>
-      <c r="P52" s="146"/>
+      <c r="N52" s="216"/>
+      <c r="O52" s="216"/>
+      <c r="P52" s="217"/>
     </row>
     <row r="53" spans="1:16" s="76" customFormat="1" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="67"/>
@@ -8735,12 +8738,12 @@
       <c r="L53" s="87" t="s">
         <v>384</v>
       </c>
-      <c r="M53" s="145" t="s">
+      <c r="M53" s="216" t="s">
         <v>385</v>
       </c>
-      <c r="N53" s="145"/>
-      <c r="O53" s="145"/>
-      <c r="P53" s="146"/>
+      <c r="N53" s="216"/>
+      <c r="O53" s="216"/>
+      <c r="P53" s="217"/>
     </row>
     <row r="54" spans="1:16" s="18" customFormat="1" ht="186.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
@@ -8778,11 +8781,11 @@
       <c r="K54" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="L54" s="202" t="s">
+      <c r="L54" s="173" t="s">
         <v>251</v>
       </c>
-      <c r="M54" s="203"/>
-      <c r="N54" s="204"/>
+      <c r="M54" s="174"/>
+      <c r="N54" s="175"/>
       <c r="O54" s="39" t="s">
         <v>252</v>
       </c>
@@ -8878,15 +8881,15 @@
       <c r="K56" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="L56" s="116" t="s">
+      <c r="L56" s="178" t="s">
         <v>490</v>
       </c>
-      <c r="M56" s="117"/>
-      <c r="N56" s="118"/>
-      <c r="O56" s="142" t="s">
+      <c r="M56" s="168"/>
+      <c r="N56" s="179"/>
+      <c r="O56" s="135" t="s">
         <v>491</v>
       </c>
-      <c r="P56" s="125" t="s">
+      <c r="P56" s="149" t="s">
         <v>489</v>
       </c>
     </row>
@@ -8926,11 +8929,11 @@
       <c r="K57" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="L57" s="119"/>
-      <c r="M57" s="120"/>
-      <c r="N57" s="121"/>
-      <c r="O57" s="143"/>
-      <c r="P57" s="126"/>
+      <c r="L57" s="223"/>
+      <c r="M57" s="169"/>
+      <c r="N57" s="224"/>
+      <c r="O57" s="215"/>
+      <c r="P57" s="150"/>
     </row>
     <row r="58" spans="1:16" s="18" customFormat="1" ht="99.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
@@ -8968,11 +8971,11 @@
       <c r="K58" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="L58" s="122"/>
-      <c r="M58" s="123"/>
-      <c r="N58" s="124"/>
-      <c r="O58" s="144"/>
-      <c r="P58" s="127"/>
+      <c r="L58" s="185"/>
+      <c r="M58" s="201"/>
+      <c r="N58" s="186"/>
+      <c r="O58" s="199"/>
+      <c r="P58" s="200"/>
     </row>
     <row r="59" spans="1:16" s="18" customFormat="1" ht="282" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
@@ -9010,10 +9013,10 @@
       <c r="K59" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="L59" s="205" t="s">
+      <c r="L59" s="176" t="s">
         <v>221</v>
       </c>
-      <c r="M59" s="206"/>
+      <c r="M59" s="177"/>
       <c r="N59" s="41" t="s">
         <v>230</v>
       </c>
@@ -9060,10 +9063,10 @@
       <c r="K60" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="L60" s="116" t="s">
+      <c r="L60" s="178" t="s">
         <v>214</v>
       </c>
-      <c r="M60" s="118"/>
+      <c r="M60" s="179"/>
       <c r="N60" s="41" t="s">
         <v>213</v>
       </c>
@@ -9110,19 +9113,19 @@
       <c r="K61" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="L61" s="194" t="s">
+      <c r="L61" s="152" t="s">
         <v>492</v>
       </c>
-      <c r="M61" s="111" t="s">
+      <c r="M61" s="154" t="s">
         <v>493</v>
       </c>
-      <c r="N61" s="114" t="s">
+      <c r="N61" s="156" t="s">
         <v>494</v>
       </c>
-      <c r="O61" s="198" t="s">
+      <c r="O61" s="120" t="s">
         <v>495</v>
       </c>
-      <c r="P61" s="200" t="s">
+      <c r="P61" s="123" t="s">
         <v>496</v>
       </c>
     </row>
@@ -9162,11 +9165,11 @@
       <c r="K62" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="L62" s="194"/>
-      <c r="M62" s="111"/>
-      <c r="N62" s="114"/>
-      <c r="O62" s="198"/>
-      <c r="P62" s="200"/>
+      <c r="L62" s="152"/>
+      <c r="M62" s="154"/>
+      <c r="N62" s="156"/>
+      <c r="O62" s="120"/>
+      <c r="P62" s="123"/>
     </row>
     <row r="63" spans="1:16" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
@@ -9204,11 +9207,11 @@
       <c r="K63" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L63" s="194"/>
-      <c r="M63" s="111"/>
-      <c r="N63" s="114"/>
-      <c r="O63" s="198"/>
-      <c r="P63" s="200"/>
+      <c r="L63" s="152"/>
+      <c r="M63" s="154"/>
+      <c r="N63" s="156"/>
+      <c r="O63" s="120"/>
+      <c r="P63" s="123"/>
     </row>
     <row r="64" spans="1:16" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
@@ -9246,11 +9249,11 @@
       <c r="K64" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L64" s="195"/>
-      <c r="M64" s="196"/>
-      <c r="N64" s="197"/>
-      <c r="O64" s="199"/>
-      <c r="P64" s="201"/>
+      <c r="L64" s="153"/>
+      <c r="M64" s="155"/>
+      <c r="N64" s="157"/>
+      <c r="O64" s="158"/>
+      <c r="P64" s="159"/>
     </row>
     <row r="65" spans="1:17" s="76" customFormat="1" ht="51.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A65" s="67" t="s">
@@ -9276,19 +9279,19 @@
       <c r="K65" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="L65" s="166" t="s">
+      <c r="L65" s="193" t="s">
         <v>497</v>
       </c>
-      <c r="M65" s="110" t="s">
+      <c r="M65" s="195" t="s">
         <v>499</v>
       </c>
-      <c r="N65" s="113" t="s">
+      <c r="N65" s="197" t="s">
         <v>500</v>
       </c>
-      <c r="O65" s="177" t="s">
+      <c r="O65" s="119" t="s">
         <v>501</v>
       </c>
-      <c r="P65" s="179" t="s">
+      <c r="P65" s="122" t="s">
         <v>498</v>
       </c>
     </row>
@@ -9316,11 +9319,11 @@
       <c r="K66" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="L66" s="167"/>
-      <c r="M66" s="112"/>
-      <c r="N66" s="115"/>
-      <c r="O66" s="178"/>
-      <c r="P66" s="180"/>
+      <c r="L66" s="194"/>
+      <c r="M66" s="196"/>
+      <c r="N66" s="198"/>
+      <c r="O66" s="121"/>
+      <c r="P66" s="124"/>
     </row>
     <row r="67" spans="1:17" ht="192" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
@@ -9358,13 +9361,13 @@
       <c r="K67" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L67" s="174" t="s">
+      <c r="L67" s="170" t="s">
         <v>201</v>
       </c>
-      <c r="M67" s="175"/>
-      <c r="N67" s="175"/>
-      <c r="O67" s="175"/>
-      <c r="P67" s="176"/>
+      <c r="M67" s="171"/>
+      <c r="N67" s="171"/>
+      <c r="O67" s="171"/>
+      <c r="P67" s="172"/>
     </row>
     <row r="68" spans="1:17" ht="90.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
@@ -9402,19 +9405,19 @@
       <c r="K68" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L68" s="166" t="s">
+      <c r="L68" s="193" t="s">
         <v>502</v>
       </c>
-      <c r="M68" s="110" t="s">
+      <c r="M68" s="195" t="s">
         <v>503</v>
       </c>
-      <c r="N68" s="113" t="s">
+      <c r="N68" s="197" t="s">
         <v>504</v>
       </c>
-      <c r="O68" s="177" t="s">
+      <c r="O68" s="119" t="s">
         <v>505</v>
       </c>
-      <c r="P68" s="179" t="s">
+      <c r="P68" s="122" t="s">
         <v>506</v>
       </c>
     </row>
@@ -9454,11 +9457,11 @@
       <c r="K69" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L69" s="181"/>
-      <c r="M69" s="111"/>
-      <c r="N69" s="114"/>
-      <c r="O69" s="198"/>
-      <c r="P69" s="200"/>
+      <c r="L69" s="206"/>
+      <c r="M69" s="154"/>
+      <c r="N69" s="156"/>
+      <c r="O69" s="120"/>
+      <c r="P69" s="123"/>
       <c r="Q69" s="16"/>
     </row>
     <row r="70" spans="1:17" s="13" customFormat="1" ht="68.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -9497,11 +9500,11 @@
       <c r="K70" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L70" s="181"/>
-      <c r="M70" s="111"/>
-      <c r="N70" s="114"/>
-      <c r="O70" s="198"/>
-      <c r="P70" s="200"/>
+      <c r="L70" s="206"/>
+      <c r="M70" s="154"/>
+      <c r="N70" s="156"/>
+      <c r="O70" s="120"/>
+      <c r="P70" s="123"/>
       <c r="Q70" s="16"/>
     </row>
     <row r="71" spans="1:17" s="13" customFormat="1" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9540,11 +9543,11 @@
       <c r="K71" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L71" s="167"/>
-      <c r="M71" s="112"/>
-      <c r="N71" s="115"/>
-      <c r="O71" s="178"/>
-      <c r="P71" s="180"/>
+      <c r="L71" s="194"/>
+      <c r="M71" s="196"/>
+      <c r="N71" s="198"/>
+      <c r="O71" s="121"/>
+      <c r="P71" s="124"/>
     </row>
     <row r="72" spans="1:17" s="13" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
@@ -9582,13 +9585,13 @@
       <c r="K72" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L72" s="171" t="s">
+      <c r="L72" s="140" t="s">
         <v>201</v>
       </c>
-      <c r="M72" s="172"/>
-      <c r="N72" s="172"/>
-      <c r="O72" s="172"/>
-      <c r="P72" s="173"/>
+      <c r="M72" s="141"/>
+      <c r="N72" s="141"/>
+      <c r="O72" s="141"/>
+      <c r="P72" s="142"/>
     </row>
     <row r="73" spans="1:17" ht="153.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
@@ -9626,11 +9629,11 @@
       <c r="K73" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L73" s="174"/>
-      <c r="M73" s="175"/>
-      <c r="N73" s="175"/>
-      <c r="O73" s="175"/>
-      <c r="P73" s="176"/>
+      <c r="L73" s="170"/>
+      <c r="M73" s="171"/>
+      <c r="N73" s="171"/>
+      <c r="O73" s="171"/>
+      <c r="P73" s="172"/>
       <c r="Q73" s="13"/>
     </row>
     <row r="74" spans="1:17" ht="102.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -9669,17 +9672,17 @@
       <c r="K74" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L74" s="116" t="s">
+      <c r="L74" s="178" t="s">
         <v>507</v>
       </c>
-      <c r="M74" s="118"/>
-      <c r="N74" s="150" t="s">
+      <c r="M74" s="179"/>
+      <c r="N74" s="137" t="s">
         <v>508</v>
       </c>
-      <c r="O74" s="142" t="s">
+      <c r="O74" s="135" t="s">
         <v>509</v>
       </c>
-      <c r="P74" s="125" t="s">
+      <c r="P74" s="149" t="s">
         <v>510</v>
       </c>
     </row>
@@ -9719,11 +9722,11 @@
       <c r="K75" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L75" s="122"/>
-      <c r="M75" s="124"/>
-      <c r="N75" s="151"/>
-      <c r="O75" s="144"/>
-      <c r="P75" s="127"/>
+      <c r="L75" s="185"/>
+      <c r="M75" s="186"/>
+      <c r="N75" s="139"/>
+      <c r="O75" s="199"/>
+      <c r="P75" s="200"/>
     </row>
     <row r="76" spans="1:17" ht="104.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
@@ -9813,13 +9816,13 @@
       <c r="K77" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L77" s="171" t="s">
+      <c r="L77" s="140" t="s">
         <v>201</v>
       </c>
-      <c r="M77" s="172"/>
-      <c r="N77" s="172"/>
-      <c r="O77" s="172"/>
-      <c r="P77" s="173"/>
+      <c r="M77" s="141"/>
+      <c r="N77" s="141"/>
+      <c r="O77" s="141"/>
+      <c r="P77" s="142"/>
     </row>
     <row r="78" spans="1:17" ht="200.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
@@ -9860,12 +9863,12 @@
       <c r="L78" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="M78" s="140" t="s">
+      <c r="M78" s="143" t="s">
         <v>231</v>
       </c>
-      <c r="N78" s="224"/>
-      <c r="O78" s="224"/>
-      <c r="P78" s="141"/>
+      <c r="N78" s="144"/>
+      <c r="O78" s="144"/>
+      <c r="P78" s="145"/>
     </row>
     <row r="79" spans="1:17" ht="243.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
@@ -9903,15 +9906,15 @@
       <c r="K79" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="L79" s="147" t="s">
+      <c r="L79" s="133" t="s">
         <v>517</v>
       </c>
-      <c r="M79" s="148"/>
-      <c r="N79" s="149"/>
-      <c r="O79" s="185" t="s">
+      <c r="M79" s="205"/>
+      <c r="N79" s="134"/>
+      <c r="O79" s="125" t="s">
         <v>518</v>
       </c>
-      <c r="P79" s="186"/>
+      <c r="P79" s="126"/>
     </row>
     <row r="80" spans="1:17" ht="218.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
@@ -9949,15 +9952,15 @@
       <c r="K80" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="L80" s="147" t="s">
+      <c r="L80" s="133" t="s">
         <v>519</v>
       </c>
-      <c r="M80" s="148"/>
-      <c r="N80" s="149"/>
-      <c r="O80" s="185" t="s">
+      <c r="M80" s="205"/>
+      <c r="N80" s="134"/>
+      <c r="O80" s="125" t="s">
         <v>520</v>
       </c>
-      <c r="P80" s="186"/>
+      <c r="P80" s="126"/>
     </row>
     <row r="81" spans="1:1024" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
@@ -9995,15 +9998,15 @@
       <c r="K81" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="L81" s="116" t="s">
+      <c r="L81" s="178" t="s">
         <v>224</v>
       </c>
-      <c r="M81" s="117"/>
-      <c r="N81" s="118"/>
-      <c r="O81" s="185" t="s">
+      <c r="M81" s="168"/>
+      <c r="N81" s="179"/>
+      <c r="O81" s="125" t="s">
         <v>521</v>
       </c>
-      <c r="P81" s="186"/>
+      <c r="P81" s="126"/>
     </row>
     <row r="82" spans="1:1024" ht="294" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
@@ -10041,11 +10044,11 @@
       <c r="K82" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="L82" s="122"/>
-      <c r="M82" s="123"/>
-      <c r="N82" s="124"/>
-      <c r="O82" s="220"/>
-      <c r="P82" s="221"/>
+      <c r="L82" s="185"/>
+      <c r="M82" s="201"/>
+      <c r="N82" s="186"/>
+      <c r="O82" s="131"/>
+      <c r="P82" s="132"/>
     </row>
     <row r="83" spans="1:1024" ht="150" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
@@ -10083,10 +10086,10 @@
       <c r="K83" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="L83" s="147" t="s">
+      <c r="L83" s="133" t="s">
         <v>225</v>
       </c>
-      <c r="M83" s="149"/>
+      <c r="M83" s="134"/>
       <c r="N83" s="36" t="s">
         <v>226</v>
       </c>
@@ -10128,10 +10131,10 @@
         <v>7</v>
       </c>
       <c r="K84" s="61"/>
-      <c r="L84" s="168"/>
-      <c r="M84" s="169"/>
-      <c r="N84" s="169"/>
-      <c r="O84" s="170"/>
+      <c r="L84" s="202"/>
+      <c r="M84" s="203"/>
+      <c r="N84" s="203"/>
+      <c r="O84" s="204"/>
       <c r="P84" s="86" t="s">
         <v>522</v>
       </c>
@@ -11180,19 +11183,19 @@
       <c r="K85" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="L85" s="154" t="s">
+      <c r="L85" s="129" t="s">
         <v>525</v>
       </c>
-      <c r="M85" s="152" t="s">
+      <c r="M85" s="127" t="s">
         <v>526</v>
       </c>
-      <c r="N85" s="150" t="s">
+      <c r="N85" s="137" t="s">
         <v>527</v>
       </c>
-      <c r="O85" s="142" t="s">
+      <c r="O85" s="135" t="s">
         <v>523</v>
       </c>
-      <c r="P85" s="125" t="s">
+      <c r="P85" s="149" t="s">
         <v>524</v>
       </c>
     </row>
@@ -11232,11 +11235,11 @@
       <c r="K86" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="L86" s="219"/>
-      <c r="M86" s="218"/>
-      <c r="N86" s="223"/>
-      <c r="O86" s="222"/>
-      <c r="P86" s="126"/>
+      <c r="L86" s="130"/>
+      <c r="M86" s="128"/>
+      <c r="N86" s="138"/>
+      <c r="O86" s="136"/>
+      <c r="P86" s="150"/>
     </row>
     <row r="87" spans="1:1024" s="77" customFormat="1" ht="198.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="67" t="s">
@@ -11258,13 +11261,13 @@
       </c>
       <c r="J87" s="79"/>
       <c r="K87" s="79"/>
-      <c r="L87" s="163" t="s">
+      <c r="L87" s="146" t="s">
         <v>389</v>
       </c>
-      <c r="M87" s="164"/>
-      <c r="N87" s="164"/>
-      <c r="O87" s="164"/>
-      <c r="P87" s="165"/>
+      <c r="M87" s="147"/>
+      <c r="N87" s="147"/>
+      <c r="O87" s="147"/>
+      <c r="P87" s="148"/>
     </row>
     <row r="88" spans="1:1024" s="77" customFormat="1" ht="234.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="67" t="s">
@@ -11302,13 +11305,13 @@
       <c r="K88" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="L88" s="163" t="s">
+      <c r="L88" s="146" t="s">
         <v>389</v>
       </c>
-      <c r="M88" s="164"/>
-      <c r="N88" s="164"/>
-      <c r="O88" s="164"/>
-      <c r="P88" s="165"/>
+      <c r="M88" s="147"/>
+      <c r="N88" s="147"/>
+      <c r="O88" s="147"/>
+      <c r="P88" s="148"/>
     </row>
     <row r="89" spans="1:1024" s="18" customFormat="1" ht="153" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
@@ -11499,13 +11502,13 @@
       </c>
       <c r="J93" s="26"/>
       <c r="K93" s="26"/>
-      <c r="L93" s="209" t="s">
+      <c r="L93" s="110" t="s">
         <v>201</v>
       </c>
-      <c r="M93" s="210"/>
-      <c r="N93" s="210"/>
-      <c r="O93" s="210"/>
-      <c r="P93" s="211"/>
+      <c r="M93" s="111"/>
+      <c r="N93" s="111"/>
+      <c r="O93" s="111"/>
+      <c r="P93" s="112"/>
     </row>
     <row r="94" spans="1:1024" ht="228" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
@@ -11543,11 +11546,11 @@
       <c r="K94" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="L94" s="212"/>
-      <c r="M94" s="213"/>
-      <c r="N94" s="213"/>
-      <c r="O94" s="213"/>
-      <c r="P94" s="214"/>
+      <c r="L94" s="113"/>
+      <c r="M94" s="114"/>
+      <c r="N94" s="114"/>
+      <c r="O94" s="114"/>
+      <c r="P94" s="115"/>
     </row>
     <row r="95" spans="1:1024" s="76" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="67" t="s">
@@ -11585,11 +11588,11 @@
       <c r="K95" s="79" t="s">
         <v>172</v>
       </c>
-      <c r="L95" s="212"/>
-      <c r="M95" s="213"/>
-      <c r="N95" s="213"/>
-      <c r="O95" s="213"/>
-      <c r="P95" s="214"/>
+      <c r="L95" s="113"/>
+      <c r="M95" s="114"/>
+      <c r="N95" s="114"/>
+      <c r="O95" s="114"/>
+      <c r="P95" s="115"/>
     </row>
     <row r="96" spans="1:1024" ht="221.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
@@ -11627,11 +11630,11 @@
       <c r="K96" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="L96" s="212"/>
-      <c r="M96" s="213"/>
-      <c r="N96" s="213"/>
-      <c r="O96" s="213"/>
-      <c r="P96" s="214"/>
+      <c r="L96" s="113"/>
+      <c r="M96" s="114"/>
+      <c r="N96" s="114"/>
+      <c r="O96" s="114"/>
+      <c r="P96" s="115"/>
     </row>
     <row r="97" spans="1:17" ht="273.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
@@ -11669,11 +11672,11 @@
       <c r="K97" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="L97" s="212"/>
-      <c r="M97" s="213"/>
-      <c r="N97" s="213"/>
-      <c r="O97" s="213"/>
-      <c r="P97" s="214"/>
+      <c r="L97" s="113"/>
+      <c r="M97" s="114"/>
+      <c r="N97" s="114"/>
+      <c r="O97" s="114"/>
+      <c r="P97" s="115"/>
     </row>
     <row r="98" spans="1:17" ht="234" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
@@ -11711,11 +11714,11 @@
       <c r="K98" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="L98" s="215"/>
-      <c r="M98" s="216"/>
-      <c r="N98" s="216"/>
-      <c r="O98" s="216"/>
-      <c r="P98" s="217"/>
+      <c r="L98" s="116"/>
+      <c r="M98" s="117"/>
+      <c r="N98" s="117"/>
+      <c r="O98" s="117"/>
+      <c r="P98" s="118"/>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="Q99" s="18"/>
@@ -11726,6 +11729,69 @@
   </sheetData>
   <autoFilter ref="A1:K98"/>
   <mergeCells count="79">
+    <mergeCell ref="M68:M71"/>
+    <mergeCell ref="N68:N71"/>
+    <mergeCell ref="L56:N58"/>
+    <mergeCell ref="P56:P58"/>
+    <mergeCell ref="O48:O49"/>
+    <mergeCell ref="P48:P49"/>
+    <mergeCell ref="L13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="O56:O58"/>
+    <mergeCell ref="M52:P52"/>
+    <mergeCell ref="M53:P53"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="L35:O35"/>
+    <mergeCell ref="P32:P33"/>
+    <mergeCell ref="O32:O33"/>
+    <mergeCell ref="N32:N33"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="L38:P38"/>
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="N48:N49"/>
+    <mergeCell ref="L87:P87"/>
+    <mergeCell ref="L65:L66"/>
+    <mergeCell ref="M65:M66"/>
+    <mergeCell ref="N65:N66"/>
+    <mergeCell ref="O74:O75"/>
+    <mergeCell ref="P74:P75"/>
+    <mergeCell ref="L81:N82"/>
+    <mergeCell ref="L84:O84"/>
+    <mergeCell ref="L72:P73"/>
+    <mergeCell ref="L67:P67"/>
+    <mergeCell ref="L79:N79"/>
+    <mergeCell ref="L80:N80"/>
+    <mergeCell ref="L74:M75"/>
+    <mergeCell ref="O65:O66"/>
+    <mergeCell ref="P65:P66"/>
+    <mergeCell ref="L68:L71"/>
+    <mergeCell ref="L41:P41"/>
+    <mergeCell ref="L48:L49"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="L39:M40"/>
+    <mergeCell ref="O39:P40"/>
+    <mergeCell ref="P44:P45"/>
+    <mergeCell ref="O44:O45"/>
+    <mergeCell ref="N44:N45"/>
+    <mergeCell ref="M44:M45"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="L61:L64"/>
+    <mergeCell ref="M61:M64"/>
+    <mergeCell ref="N61:N64"/>
+    <mergeCell ref="O61:O64"/>
+    <mergeCell ref="P61:P64"/>
+    <mergeCell ref="P46:P47"/>
+    <mergeCell ref="O46:O47"/>
+    <mergeCell ref="N46:N47"/>
+    <mergeCell ref="M46:M47"/>
+    <mergeCell ref="L46:L47"/>
+    <mergeCell ref="L30:P31"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="L59:M59"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="L44:L45"/>
     <mergeCell ref="L93:P98"/>
     <mergeCell ref="O68:O71"/>
     <mergeCell ref="P68:P71"/>
@@ -11742,69 +11808,6 @@
     <mergeCell ref="M78:P78"/>
     <mergeCell ref="L88:P88"/>
     <mergeCell ref="P85:P86"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="L61:L64"/>
-    <mergeCell ref="M61:M64"/>
-    <mergeCell ref="N61:N64"/>
-    <mergeCell ref="O61:O64"/>
-    <mergeCell ref="P61:P64"/>
-    <mergeCell ref="P46:P47"/>
-    <mergeCell ref="O46:O47"/>
-    <mergeCell ref="N46:N47"/>
-    <mergeCell ref="M46:M47"/>
-    <mergeCell ref="L46:L47"/>
-    <mergeCell ref="L30:P31"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="L59:M59"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="L44:L45"/>
-    <mergeCell ref="L41:P41"/>
-    <mergeCell ref="L48:L49"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="L39:M40"/>
-    <mergeCell ref="O39:P40"/>
-    <mergeCell ref="P44:P45"/>
-    <mergeCell ref="O44:O45"/>
-    <mergeCell ref="N44:N45"/>
-    <mergeCell ref="M44:M45"/>
-    <mergeCell ref="L87:P87"/>
-    <mergeCell ref="L65:L66"/>
-    <mergeCell ref="M65:M66"/>
-    <mergeCell ref="N65:N66"/>
-    <mergeCell ref="O74:O75"/>
-    <mergeCell ref="P74:P75"/>
-    <mergeCell ref="L81:N82"/>
-    <mergeCell ref="L84:O84"/>
-    <mergeCell ref="L72:P73"/>
-    <mergeCell ref="L67:P67"/>
-    <mergeCell ref="L79:N79"/>
-    <mergeCell ref="L80:N80"/>
-    <mergeCell ref="L74:M75"/>
-    <mergeCell ref="O65:O66"/>
-    <mergeCell ref="P65:P66"/>
-    <mergeCell ref="L68:L71"/>
-    <mergeCell ref="L13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="O56:O58"/>
-    <mergeCell ref="M52:P52"/>
-    <mergeCell ref="M53:P53"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="L35:O35"/>
-    <mergeCell ref="P32:P33"/>
-    <mergeCell ref="O32:O33"/>
-    <mergeCell ref="N32:N33"/>
-    <mergeCell ref="M32:M33"/>
-    <mergeCell ref="L32:L33"/>
-    <mergeCell ref="L38:P38"/>
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="N48:N49"/>
-    <mergeCell ref="M68:M71"/>
-    <mergeCell ref="N68:N71"/>
-    <mergeCell ref="L56:N58"/>
-    <mergeCell ref="P56:P58"/>
-    <mergeCell ref="O48:O49"/>
-    <mergeCell ref="P48:P49"/>
   </mergeCells>
   <conditionalFormatting sqref="H61:H62">
     <cfRule type="duplicateValues" dxfId="3" priority="20"/>
@@ -11816,11 +11819,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="109" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="109" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11869,7 +11871,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="76.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
         <v>161</v>
       </c>
@@ -11887,7 +11889,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="67"/>
       <c r="B3" s="67"/>
       <c r="C3" s="67"/>
@@ -11903,7 +11905,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="B4" s="67"/>
       <c r="C4" s="67"/>
@@ -11919,7 +11921,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="280.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="280.5" x14ac:dyDescent="0.25">
       <c r="A5" s="67"/>
       <c r="B5" s="67"/>
       <c r="C5" s="67"/>
@@ -11939,7 +11941,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="67"/>
       <c r="B6" s="67"/>
       <c r="C6" s="67"/>
@@ -11959,7 +11961,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="67"/>
       <c r="B7" s="67"/>
       <c r="C7" s="67"/>
@@ -11979,7 +11981,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="67"/>
       <c r="B8" s="67"/>
       <c r="C8" s="67"/>
@@ -11999,7 +12001,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="67"/>
       <c r="B9" s="67"/>
       <c r="C9" s="67"/>
@@ -12019,7 +12021,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="67" t="s">
         <v>534</v>
       </c>
@@ -12041,7 +12043,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="67"/>
       <c r="B11" s="67"/>
       <c r="C11" s="67"/>
@@ -12061,7 +12063,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="67"/>
       <c r="B12" s="67"/>
       <c r="C12" s="67"/>
@@ -12081,7 +12083,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="67"/>
       <c r="B13" s="67"/>
       <c r="C13" s="67"/>
@@ -12101,7 +12103,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A14" s="67"/>
       <c r="B14" s="67"/>
       <c r="C14" s="67"/>
@@ -12184,7 +12186,7 @@
         <v>545</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="102" x14ac:dyDescent="0.25">
@@ -12218,10 +12220,10 @@
         <v>545</v>
       </c>
       <c r="J17" s="27" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="76.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A18" s="91" t="s">
         <v>5</v>
       </c>
@@ -12320,7 +12322,7 @@
         <v>545</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
@@ -12354,7 +12356,7 @@
         <v>545</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="102" x14ac:dyDescent="0.25">
@@ -12388,7 +12390,7 @@
         <v>545</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
@@ -12422,7 +12424,7 @@
         <v>545</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
@@ -12456,7 +12458,7 @@
         <v>545</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
@@ -12490,7 +12492,7 @@
         <v>545</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
@@ -12524,7 +12526,7 @@
         <v>545</v>
       </c>
       <c r="J26" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="51" x14ac:dyDescent="0.25">
@@ -12558,7 +12560,7 @@
         <v>545</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="191.25" x14ac:dyDescent="0.25">
@@ -12592,7 +12594,7 @@
         <v>545</v>
       </c>
       <c r="J28" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
@@ -12626,7 +12628,7 @@
         <v>545</v>
       </c>
       <c r="J29" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="191.25" x14ac:dyDescent="0.25">
@@ -12660,7 +12662,7 @@
         <v>545</v>
       </c>
       <c r="J30" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
@@ -12694,7 +12696,7 @@
         <v>545</v>
       </c>
       <c r="J31" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
@@ -12728,7 +12730,7 @@
         <v>545</v>
       </c>
       <c r="J32" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
@@ -12762,7 +12764,7 @@
         <v>545</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
@@ -12796,10 +12798,10 @@
         <v>545</v>
       </c>
       <c r="J34" s="27" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="204" hidden="1" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="204" x14ac:dyDescent="0.25">
       <c r="A35" s="91" t="s">
         <v>22</v>
       </c>
@@ -12830,7 +12832,7 @@
         <v>545</v>
       </c>
       <c r="J35" s="27" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
@@ -12864,7 +12866,7 @@
         <v>545</v>
       </c>
       <c r="J36" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="165.75" x14ac:dyDescent="0.25">
@@ -12898,7 +12900,7 @@
         <v>545</v>
       </c>
       <c r="J37" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
@@ -12966,10 +12968,10 @@
         <v>545</v>
       </c>
       <c r="J39" s="27" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="229.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="229.5" x14ac:dyDescent="0.25">
       <c r="A40" s="91" t="s">
         <v>22</v>
       </c>
@@ -13000,7 +13002,7 @@
         <v>545</v>
       </c>
       <c r="J40" s="27" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
@@ -13034,7 +13036,7 @@
         <v>545</v>
       </c>
       <c r="J41" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -13068,7 +13070,7 @@
         <v>545</v>
       </c>
       <c r="J42" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="165.75" x14ac:dyDescent="0.25">
@@ -13102,7 +13104,7 @@
         <v>545</v>
       </c>
       <c r="J43" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="165.75" x14ac:dyDescent="0.25">
@@ -13136,7 +13138,7 @@
         <v>545</v>
       </c>
       <c r="J44" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -13170,7 +13172,7 @@
         <v>545</v>
       </c>
       <c r="J45" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -13204,10 +13206,10 @@
         <v>545</v>
       </c>
       <c r="J46" s="27" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A47" s="91" t="s">
         <v>29</v>
       </c>
@@ -13238,7 +13240,7 @@
         <v>545</v>
       </c>
       <c r="J47" s="27" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -13271,8 +13273,8 @@
       <c r="I48" s="27" t="s">
         <v>545</v>
       </c>
-      <c r="J48" s="27" t="s">
-        <v>765</v>
+      <c r="J48" s="225" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="165.75" x14ac:dyDescent="0.25">
@@ -13306,7 +13308,7 @@
         <v>545</v>
       </c>
       <c r="J49" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
@@ -13340,10 +13342,10 @@
         <v>545</v>
       </c>
       <c r="J50" s="27" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A51" s="91" t="s">
         <v>29</v>
       </c>
@@ -13374,7 +13376,7 @@
         <v>545</v>
       </c>
       <c r="J51" s="27" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -13408,7 +13410,7 @@
         <v>545</v>
       </c>
       <c r="J52" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -13442,7 +13444,7 @@
         <v>545</v>
       </c>
       <c r="J53" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="153" x14ac:dyDescent="0.25">
@@ -13476,7 +13478,7 @@
         <v>545</v>
       </c>
       <c r="J54" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="51" x14ac:dyDescent="0.25">
@@ -13510,7 +13512,7 @@
         <v>545</v>
       </c>
       <c r="J55" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
@@ -13544,7 +13546,7 @@
         <v>545</v>
       </c>
       <c r="J56" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
@@ -13612,7 +13614,7 @@
         <v>545</v>
       </c>
       <c r="J58" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="306" x14ac:dyDescent="0.25">
@@ -13646,7 +13648,7 @@
         <v>545</v>
       </c>
       <c r="J59" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="216.75" x14ac:dyDescent="0.25">
@@ -13680,7 +13682,7 @@
         <v>545</v>
       </c>
       <c r="J60" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
@@ -13714,7 +13716,7 @@
         <v>545</v>
       </c>
       <c r="J61" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
@@ -13748,10 +13750,10 @@
         <v>545</v>
       </c>
       <c r="J62" s="27" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="76.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A63" s="91" t="s">
         <v>46</v>
       </c>
@@ -13782,7 +13784,7 @@
         <v>545</v>
       </c>
       <c r="J63" s="27" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -13812,7 +13814,7 @@
         <v>545</v>
       </c>
       <c r="J64" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="140.25" x14ac:dyDescent="0.25">
@@ -13842,7 +13844,7 @@
         <v>545</v>
       </c>
       <c r="J65" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
@@ -13876,7 +13878,7 @@
         <v>545</v>
       </c>
       <c r="J66" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -13908,11 +13910,11 @@
       <c r="I67" s="27" t="s">
         <v>545</v>
       </c>
-      <c r="J67" s="27" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J67" s="225" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A68" s="91" t="s">
         <v>47</v>
       </c>
@@ -13943,10 +13945,10 @@
         <v>545</v>
       </c>
       <c r="J68" s="27" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A69" s="91" t="s">
         <v>47</v>
       </c>
@@ -13977,7 +13979,7 @@
         <v>545</v>
       </c>
       <c r="J69" s="27" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -14011,10 +14013,10 @@
         <v>545</v>
       </c>
       <c r="J70" s="27" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A71" s="91" t="s">
         <v>47</v>
       </c>
@@ -14045,10 +14047,10 @@
         <v>545</v>
       </c>
       <c r="J71" s="27" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="89.25" hidden="1" x14ac:dyDescent="0.25">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A72" s="91" t="s">
         <v>92</v>
       </c>
@@ -14079,10 +14081,10 @@
         <v>545</v>
       </c>
       <c r="J72" s="27" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="242.25" hidden="1" x14ac:dyDescent="0.25">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A73" s="91" t="s">
         <v>92</v>
       </c>
@@ -14113,10 +14115,10 @@
         <v>545</v>
       </c>
       <c r="J73" s="27" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="242.25" hidden="1" x14ac:dyDescent="0.25">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A74" s="91" t="s">
         <v>92</v>
       </c>
@@ -14147,10 +14149,10 @@
         <v>545</v>
       </c>
       <c r="J74" s="27" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.25">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A75" s="91" t="s">
         <v>92</v>
       </c>
@@ -14181,7 +14183,7 @@
         <v>545</v>
       </c>
       <c r="J75" s="27" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="280.5" x14ac:dyDescent="0.25">
@@ -14218,7 +14220,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A77" s="91" t="s">
         <v>92</v>
       </c>
@@ -14249,7 +14251,7 @@
         <v>545</v>
       </c>
       <c r="J77" s="27" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="140.25" x14ac:dyDescent="0.25">
@@ -14317,10 +14319,10 @@
         <v>545</v>
       </c>
       <c r="J79" s="27" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A80" s="91" t="s">
         <v>92</v>
       </c>
@@ -14351,10 +14353,10 @@
         <v>545</v>
       </c>
       <c r="J80" s="27" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="51" hidden="1" x14ac:dyDescent="0.25">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A81" s="91" t="s">
         <v>92</v>
       </c>
@@ -14385,7 +14387,7 @@
         <v>545</v>
       </c>
       <c r="J81" s="27" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -14419,7 +14421,7 @@
         <v>545</v>
       </c>
       <c r="J82" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="102" x14ac:dyDescent="0.25">
@@ -14453,7 +14455,7 @@
         <v>545</v>
       </c>
       <c r="J83" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
@@ -14483,7 +14485,7 @@
         <v>545</v>
       </c>
       <c r="J84" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="140.25" x14ac:dyDescent="0.25">
@@ -14517,7 +14519,7 @@
         <v>545</v>
       </c>
       <c r="J85" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -14551,7 +14553,7 @@
         <v>545</v>
       </c>
       <c r="J86" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -14585,7 +14587,7 @@
         <v>545</v>
       </c>
       <c r="J87" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -14619,7 +14621,7 @@
         <v>545</v>
       </c>
       <c r="J88" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
@@ -14653,7 +14655,7 @@
         <v>545</v>
       </c>
       <c r="J89" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="344.25" x14ac:dyDescent="0.25">
@@ -14687,7 +14689,7 @@
         <v>545</v>
       </c>
       <c r="J90" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="255" x14ac:dyDescent="0.25">
@@ -14721,7 +14723,7 @@
         <v>545</v>
       </c>
       <c r="J91" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="140.25" x14ac:dyDescent="0.25">
@@ -14755,7 +14757,7 @@
         <v>545</v>
       </c>
       <c r="J92" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="382.5" x14ac:dyDescent="0.25">
@@ -14823,7 +14825,7 @@
         <v>545</v>
       </c>
       <c r="J94" s="27" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
@@ -15879,14 +15881,7 @@
       <c r="I217" s="106"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J95">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="Choix multiple: Toutes les réponses sont égales (pondération modale)"/>
-        <filter val="Toutes les réponses sont égales (pondération modale)"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J95"/>
   <conditionalFormatting sqref="G27">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>

</xml_diff>